<commit_message>
Update platform restrrictions for cell
</commit_message>
<xml_diff>
--- a/workbooks/CommsDatabase3.xlsx
+++ b/workbooks/CommsDatabase3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Dropbox\PMASE - Capstone\Solution Design\Tech Matrices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkeller6\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>9,13</t>
+  </si>
+  <si>
+    <t>3,6,7,8</t>
   </si>
 </sst>
 </file>
@@ -689,7 +692,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +972,9 @@
       <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -1000,7 +1005,9 @@
       <c r="D9" s="4">
         <v>1</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>

</xml_diff>